<commit_message>
Added new students and removed raija from group info
</commit_message>
<xml_diff>
--- a/website_content_creation/authors/Raija_Hache/Hache_Author_form.xlsx
+++ b/website_content_creation/authors/Raija_Hache/Hache_Author_form.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://041gc-my.sharepoint.com/personal/emily_smenderovac_nrcan-rncan_gc_ca/Documents/Documents/WET lab/GLFC-WET.github.io/website_content_creation/authors/Raija_Hache/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{E84AE7BC-A86C-4F86-93BA-F0F421642BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13706494-B963-49F4-B74D-D8B89B412758}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{E84AE7BC-A86C-4F86-93BA-F0F421642BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{929BE797-6BA5-46BD-88B5-67C6335ED6F2}"/>
   <bookViews>
-    <workbookView xWindow="-12765" yWindow="-15045" windowWidth="27000" windowHeight="14385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20790" yWindow="-13605" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,7 @@
     <t>Environmental Technologist</t>
   </si>
   <si>
-    <t>Watershed Ecology Team</t>
+    <t>Past WETlab Members</t>
   </si>
 </sst>
 </file>
@@ -798,7 +798,7 @@
   <dimension ref="A1:C1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>